<commit_message>
Updated gerb and JLC bom
</commit_message>
<xml_diff>
--- a/polygonus-Shortage-Version/export/v0.2/JLCBOM-Fixed.xlsx
+++ b/polygonus-Shortage-Version/export/v0.2/JLCBOM-Fixed.xlsx
@@ -434,15 +434,9 @@
     <t>C7975</t>
   </si>
   <si>
-    <t>STM32F429ZGTx</t>
-  </si>
-  <si>
     <t>Package_QFP:LQFP-144_20x20mm_P0.5mm</t>
   </si>
   <si>
-    <t>C91685</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:SOT-323_SC-70</t>
   </si>
   <si>
@@ -651,6 +645,12 @@
   </si>
   <si>
     <t>C543679</t>
+  </si>
+  <si>
+    <t>STM32F407ZGTx</t>
+  </si>
+  <si>
+    <t>C19156</t>
   </si>
 </sst>
 </file>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1006,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,10 +1020,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,10 +1034,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,10 +1062,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,10 +1076,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,10 +1090,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,10 +1104,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,10 +1132,10 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,10 +1146,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,10 +1160,10 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" t="s">
         <v>147</v>
-      </c>
-      <c r="D13" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,24 +1174,24 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,10 +1202,10 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,10 +1216,10 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,10 +1230,10 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,10 +1258,10 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,10 +1300,10 @@
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,10 +1328,10 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,10 +1384,10 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,10 +1398,10 @@
         <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,10 +1412,10 @@
         <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,10 +1440,10 @@
         <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,10 +1454,10 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,10 +1468,10 @@
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,10 +1482,10 @@
         <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,10 +1496,10 @@
         <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,10 +1510,10 @@
         <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,15 +1538,15 @@
         <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
         <v>75</v>
@@ -1566,10 +1566,10 @@
         <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,10 +1580,10 @@
         <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,10 +1594,10 @@
         <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,10 +1608,10 @@
         <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,10 +1622,10 @@
         <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1636,10 +1636,10 @@
         <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,24 +1650,24 @@
         <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
         <v>88</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,10 +1678,10 @@
         <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,10 +1692,10 @@
         <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,10 +1706,10 @@
         <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,10 +1720,10 @@
         <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>98</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>101</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>104</v>
       </c>
       <c r="D56" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>53</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>21</v>
       </c>
       <c r="D58" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>89</v>
       </c>
       <c r="D60" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>110</v>
       </c>
       <c r="D62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>